<commit_message>
empty update for main prior to using real-time input filter  branch
</commit_message>
<xml_diff>
--- a/docs/resource log.xlsx
+++ b/docs/resource log.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\halog\Desktop\Music_Tutor_Project\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{904225C6-C92C-4D58-96FE-1CAD1303B910}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D55519D2-8E82-44D4-B71F-BD446B5EA63E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{41780912-9485-457E-8E39-EF1EA0B82C48}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="111">
   <si>
     <t>Date</t>
   </si>
@@ -356,6 +356,24 @@
   </si>
   <si>
     <t>stringn agg function</t>
+  </si>
+  <si>
+    <t>useSearchParams</t>
+  </si>
+  <si>
+    <t>url state</t>
+  </si>
+  <si>
+    <t>putting state in url</t>
+  </si>
+  <si>
+    <t>react search bar with filters</t>
+  </si>
+  <si>
+    <t>react with masoud</t>
+  </si>
+  <si>
+    <t>creating a real-time filter in search bar</t>
   </si>
 </sst>
 </file>
@@ -767,10 +785,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F90D4E2F-31CB-4504-B764-69927272A7DB}">
-  <dimension ref="A1:D30"/>
+  <dimension ref="A1:D32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1179,6 +1198,34 @@
       </c>
       <c r="D30" s="3" t="s">
         <v>104</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="5">
+        <v>45969</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="5">
+        <v>45972</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>110</v>
       </c>
     </row>
   </sheetData>
@@ -1212,9 +1259,11 @@
     <hyperlink ref="C28" r:id="rId26" xr:uid="{072DA101-1931-49E8-A980-D4E5DA46DA28}"/>
     <hyperlink ref="C29" r:id="rId27" xr:uid="{175426E0-1FE8-40DB-BE91-6EC5C819E87C}"/>
     <hyperlink ref="C30" r:id="rId28" xr:uid="{5A1495FF-2FD8-48B3-A242-89BA4C559C98}"/>
+    <hyperlink ref="C31" r:id="rId29" xr:uid="{5BBE4442-9BCA-44BB-886F-D6DEADB1680F}"/>
+    <hyperlink ref="C32" r:id="rId30" xr:uid="{6C3574CE-44B0-4CCE-A4AE-D9549B3F16F4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId29"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId31"/>
 </worksheet>
 </file>
 

</xml_diff>